<commit_message>
updated XDYouTube for newest version of XD-MVC and fixed some bugs
</commit_message>
<xml_diff>
--- a/User Study/Results/results.xlsx
+++ b/User Study/Results/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14235" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14235" firstSheet="5" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Total" sheetId="16" r:id="rId14"/>
     <sheet name="Comments" sheetId="20" r:id="rId15"/>
     <sheet name="Debugging strategies" sheetId="22" r:id="rId16"/>
+    <sheet name="number of devices used" sheetId="23" r:id="rId17"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="241">
   <si>
     <t>Year of birth</t>
   </si>
@@ -733,6 +734,36 @@
   <si>
     <t>Used function debugging</t>
   </si>
+  <si>
+    <t>xdcb-wo</t>
+  </si>
+  <si>
+    <t>xdci-w</t>
+  </si>
+  <si>
+    <t>xdci-wo</t>
+  </si>
+  <si>
+    <t>xdcb-w</t>
+  </si>
+  <si>
+    <t>xdytb-w</t>
+  </si>
+  <si>
+    <t>xdytb-wo</t>
+  </si>
+  <si>
+    <t>xdyti-w</t>
+  </si>
+  <si>
+    <t>xdyti-wo</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Emulated</t>
+  </si>
 </sst>
 </file>
 
@@ -1247,11 +1278,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="218204736"/>
-        <c:axId val="243399832"/>
+        <c:axId val="133605312"/>
+        <c:axId val="133606096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="218204736"/>
+        <c:axId val="133605312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,7 +1325,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243399832"/>
+        <c:crossAx val="133606096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1302,7 +1333,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243399832"/>
+        <c:axId val="133606096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1384,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218204736"/>
+        <c:crossAx val="133605312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1545,7 +1576,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1696,7 +1726,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1767,11 +1796,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="245264104"/>
-        <c:axId val="245264496"/>
+        <c:axId val="136512776"/>
+        <c:axId val="136876560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245264104"/>
+        <c:axId val="136512776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1843,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245264496"/>
+        <c:crossAx val="136876560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1822,7 +1851,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245264496"/>
+        <c:axId val="136876560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1875,7 +1904,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245264104"/>
+        <c:crossAx val="136512776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1890,7 +1919,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2154,9 +2182,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2436,7 +2462,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2699,9 +2724,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2761,7 +2784,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3025,9 +3047,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3087,7 +3107,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3351,9 +3370,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3413,7 +3430,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3677,9 +3693,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3739,7 +3753,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4009,9 +4022,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4071,7 +4082,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4451,11 +4461,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="244732896"/>
-        <c:axId val="244733288"/>
+        <c:axId val="136879696"/>
+        <c:axId val="136880088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244732896"/>
+        <c:axId val="136879696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4498,7 +4508,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244733288"/>
+        <c:crossAx val="136880088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4506,7 +4516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244733288"/>
+        <c:axId val="136880088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4558,7 +4568,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244732896"/>
+        <c:crossAx val="136879696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4572,7 +4582,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4916,11 +4925,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="244734072"/>
-        <c:axId val="244734464"/>
+        <c:axId val="136828272"/>
+        <c:axId val="136828664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244734072"/>
+        <c:axId val="136828272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4963,7 +4972,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244734464"/>
+        <c:crossAx val="136828664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4971,7 +4980,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244734464"/>
+        <c:axId val="136828664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5023,7 +5032,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244734072"/>
+        <c:crossAx val="136828272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5037,7 +5046,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5345,11 +5353,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="244735248"/>
-        <c:axId val="244735640"/>
+        <c:axId val="136829448"/>
+        <c:axId val="136829840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244735248"/>
+        <c:axId val="136829448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5392,7 +5400,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244735640"/>
+        <c:crossAx val="136829840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5400,7 +5408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244735640"/>
+        <c:axId val="136829840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -5452,7 +5460,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244735248"/>
+        <c:crossAx val="136829448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5466,7 +5474,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5894,11 +5901,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="243401008"/>
-        <c:axId val="243401400"/>
+        <c:axId val="134786104"/>
+        <c:axId val="134786496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="243401008"/>
+        <c:axId val="134786104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5941,7 +5948,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243401400"/>
+        <c:crossAx val="134786496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5949,7 +5956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243401400"/>
+        <c:axId val="134786496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6000,7 +6007,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243401008"/>
+        <c:crossAx val="134786104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6188,11 +6195,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="244736424"/>
-        <c:axId val="245059552"/>
+        <c:axId val="136830624"/>
+        <c:axId val="136831016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244736424"/>
+        <c:axId val="136830624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6235,7 +6242,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245059552"/>
+        <c:crossAx val="136831016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6243,7 +6250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245059552"/>
+        <c:axId val="136831016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -6296,7 +6303,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244736424"/>
+        <c:crossAx val="136830624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -6459,11 +6466,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="245060336"/>
-        <c:axId val="245060728"/>
+        <c:axId val="138767848"/>
+        <c:axId val="138768240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245060336"/>
+        <c:axId val="138767848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6506,7 +6513,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245060728"/>
+        <c:crossAx val="138768240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6514,7 +6521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245060728"/>
+        <c:axId val="138768240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -6567,7 +6574,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245060336"/>
+        <c:crossAx val="138767848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -7095,11 +7102,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="245061512"/>
-        <c:axId val="245061904"/>
+        <c:axId val="138769024"/>
+        <c:axId val="138769416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245061512"/>
+        <c:axId val="138769024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7142,7 +7149,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245061904"/>
+        <c:crossAx val="138769416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7150,7 +7157,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245061904"/>
+        <c:axId val="138769416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7201,7 +7208,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245061512"/>
+        <c:crossAx val="138769024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7721,11 +7728,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="245062688"/>
-        <c:axId val="245063080"/>
+        <c:axId val="138770200"/>
+        <c:axId val="138770592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245062688"/>
+        <c:axId val="138770200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7768,7 +7775,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245063080"/>
+        <c:crossAx val="138770592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7776,7 +7783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245063080"/>
+        <c:axId val="138770592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7827,7 +7834,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245062688"/>
+        <c:crossAx val="138770200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7841,7 +7848,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8033,11 +8039,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="245919752"/>
-        <c:axId val="245920144"/>
+        <c:axId val="138771376"/>
+        <c:axId val="138578368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245919752"/>
+        <c:axId val="138771376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8080,7 +8086,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245920144"/>
+        <c:crossAx val="138578368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8088,7 +8094,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245920144"/>
+        <c:axId val="138578368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -8140,7 +8146,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245919752"/>
+        <c:crossAx val="138771376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -8315,11 +8321,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="245920928"/>
-        <c:axId val="245921320"/>
+        <c:axId val="138579152"/>
+        <c:axId val="138579544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245920928"/>
+        <c:axId val="138579152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8362,7 +8368,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245921320"/>
+        <c:crossAx val="138579544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8370,7 +8376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245921320"/>
+        <c:axId val="138579544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -8422,7 +8428,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245920928"/>
+        <c:crossAx val="138579152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -8597,11 +8603,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="245922104"/>
-        <c:axId val="245922496"/>
+        <c:axId val="138580328"/>
+        <c:axId val="138580720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="245922104"/>
+        <c:axId val="138580328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8644,7 +8650,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245922496"/>
+        <c:crossAx val="138580720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8652,7 +8658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="245922496"/>
+        <c:axId val="138580720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -8704,7 +8710,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="245922104"/>
+        <c:crossAx val="138580328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -8879,11 +8885,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="246059760"/>
-        <c:axId val="246060152"/>
+        <c:axId val="138581504"/>
+        <c:axId val="138581896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246059760"/>
+        <c:axId val="138581504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8926,7 +8932,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246060152"/>
+        <c:crossAx val="138581896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8934,7 +8940,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246060152"/>
+        <c:axId val="138581896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -8986,7 +8992,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246059760"/>
+        <c:crossAx val="138581504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -9532,11 +9538,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="246060936"/>
-        <c:axId val="246061328"/>
+        <c:axId val="138722128"/>
+        <c:axId val="138722520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246060936"/>
+        <c:axId val="138722128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9579,7 +9585,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246061328"/>
+        <c:crossAx val="138722520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9587,7 +9593,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246061328"/>
+        <c:axId val="138722520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -9639,7 +9645,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246060936"/>
+        <c:crossAx val="138722128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10222,11 +10228,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="246062112"/>
-        <c:axId val="246062504"/>
+        <c:axId val="138723304"/>
+        <c:axId val="138723696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246062112"/>
+        <c:axId val="138723304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10269,7 +10275,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246062504"/>
+        <c:crossAx val="138723696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10277,7 +10283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246062504"/>
+        <c:axId val="138723696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -10329,7 +10335,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246062112"/>
+        <c:crossAx val="138723304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10631,11 +10637,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="243402184"/>
-        <c:axId val="243402576"/>
+        <c:axId val="134787280"/>
+        <c:axId val="134787672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="243402184"/>
+        <c:axId val="134787280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10678,7 +10684,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243402576"/>
+        <c:crossAx val="134787672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10686,7 +10692,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243402576"/>
+        <c:axId val="134787672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -10739,7 +10745,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243402184"/>
+        <c:crossAx val="134787280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -11320,11 +11326,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="246063288"/>
-        <c:axId val="246294600"/>
+        <c:axId val="138724480"/>
+        <c:axId val="138724872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246063288"/>
+        <c:axId val="138724480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11367,7 +11373,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246294600"/>
+        <c:crossAx val="138724872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11375,7 +11381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246294600"/>
+        <c:axId val="138724872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -11427,7 +11433,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246063288"/>
+        <c:crossAx val="138724480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12007,11 +12013,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="246295384"/>
-        <c:axId val="246295776"/>
+        <c:axId val="139015632"/>
+        <c:axId val="139016024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246295384"/>
+        <c:axId val="139015632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12054,7 +12060,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246295776"/>
+        <c:crossAx val="139016024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12062,7 +12068,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246295776"/>
+        <c:axId val="139016024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -12114,7 +12120,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246295384"/>
+        <c:crossAx val="139015632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12534,11 +12540,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="246296560"/>
-        <c:axId val="246296952"/>
+        <c:axId val="139016808"/>
+        <c:axId val="139017200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246296560"/>
+        <c:axId val="139016808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12581,7 +12587,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246296952"/>
+        <c:crossAx val="139017200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12589,7 +12595,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246296952"/>
+        <c:axId val="139017200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -12642,7 +12648,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246296560"/>
+        <c:crossAx val="139016808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -13062,11 +13068,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="246297736"/>
-        <c:axId val="246298128"/>
+        <c:axId val="139017984"/>
+        <c:axId val="139018376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246297736"/>
+        <c:axId val="139017984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13109,7 +13115,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246298128"/>
+        <c:crossAx val="139018376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13117,7 +13123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246298128"/>
+        <c:axId val="139018376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -13170,7 +13176,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246297736"/>
+        <c:crossAx val="139017984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1"/>
@@ -13590,11 +13596,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="246421984"/>
-        <c:axId val="246422376"/>
+        <c:axId val="139019160"/>
+        <c:axId val="137100008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246421984"/>
+        <c:axId val="139019160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13637,7 +13643,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246422376"/>
+        <c:crossAx val="137100008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13645,7 +13651,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246422376"/>
+        <c:axId val="137100008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -13698,7 +13704,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246421984"/>
+        <c:crossAx val="139019160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -13713,7 +13719,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14119,11 +14124,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="246423160"/>
-        <c:axId val="246423552"/>
+        <c:axId val="137100792"/>
+        <c:axId val="137101184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246423160"/>
+        <c:axId val="137100792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14166,7 +14171,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246423552"/>
+        <c:crossAx val="137101184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14174,7 +14179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246423552"/>
+        <c:axId val="137101184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -14227,7 +14232,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246423160"/>
+        <c:crossAx val="137100792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -14242,7 +14247,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14784,11 +14788,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="246424336"/>
-        <c:axId val="246424728"/>
+        <c:axId val="137101968"/>
+        <c:axId val="137102360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246424336"/>
+        <c:axId val="137101968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14831,7 +14835,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246424728"/>
+        <c:crossAx val="137102360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14839,7 +14843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246424728"/>
+        <c:axId val="137102360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14890,7 +14894,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246424336"/>
+        <c:crossAx val="137101968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14904,7 +14908,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15192,11 +15195,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="246665864"/>
-        <c:axId val="246666256"/>
+        <c:axId val="137103144"/>
+        <c:axId val="137103536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246665864"/>
+        <c:axId val="137103144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15239,7 +15242,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246666256"/>
+        <c:crossAx val="137103536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15247,7 +15250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246666256"/>
+        <c:axId val="137103536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15298,7 +15301,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246665864"/>
+        <c:crossAx val="137103144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15600,11 +15603,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="246667040"/>
-        <c:axId val="246667432"/>
+        <c:axId val="139296640"/>
+        <c:axId val="139297032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246667040"/>
+        <c:axId val="139296640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15647,7 +15650,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246667432"/>
+        <c:crossAx val="139297032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15655,7 +15658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246667432"/>
+        <c:axId val="139297032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15706,7 +15709,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246667040"/>
+        <c:crossAx val="139296640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16008,11 +16011,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="246668216"/>
-        <c:axId val="246668608"/>
+        <c:axId val="139297816"/>
+        <c:axId val="139298208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246668216"/>
+        <c:axId val="139297816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16055,7 +16058,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246668608"/>
+        <c:crossAx val="139298208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16063,7 +16066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246668608"/>
+        <c:axId val="139298208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -16116,7 +16119,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246668216"/>
+        <c:crossAx val="139297816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16418,11 +16421,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="244206720"/>
-        <c:axId val="244207112"/>
+        <c:axId val="136526032"/>
+        <c:axId val="136526424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244206720"/>
+        <c:axId val="136526032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16465,7 +16468,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244207112"/>
+        <c:crossAx val="136526424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16473,7 +16476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244207112"/>
+        <c:axId val="136526424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -16526,7 +16529,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244206720"/>
+        <c:crossAx val="136526032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -16945,11 +16948,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="244207896"/>
-        <c:axId val="244208288"/>
+        <c:axId val="136528776"/>
+        <c:axId val="136529168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244207896"/>
+        <c:axId val="136528776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16992,7 +16995,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244208288"/>
+        <c:crossAx val="136529168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17000,7 +17003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244208288"/>
+        <c:axId val="136529168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -17053,7 +17056,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244207896"/>
+        <c:crossAx val="136528776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -17472,11 +17475,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="244209072"/>
-        <c:axId val="244209464"/>
+        <c:axId val="136528384"/>
+        <c:axId val="136527992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244209072"/>
+        <c:axId val="136528384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17519,7 +17522,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244209464"/>
+        <c:crossAx val="136527992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17527,7 +17530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244209464"/>
+        <c:axId val="136527992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -17580,7 +17583,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244209072"/>
+        <c:crossAx val="136528384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1"/>
@@ -17993,11 +17996,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="244016040"/>
-        <c:axId val="244016432"/>
+        <c:axId val="136527208"/>
+        <c:axId val="136509640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244016040"/>
+        <c:axId val="136527208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18040,7 +18043,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244016432"/>
+        <c:crossAx val="136509640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18048,7 +18051,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244016432"/>
+        <c:axId val="136509640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -18101,7 +18104,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244016040"/>
+        <c:crossAx val="136527208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="1"/>
@@ -18513,11 +18516,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="244017216"/>
-        <c:axId val="244017608"/>
+        <c:axId val="136510424"/>
+        <c:axId val="136510816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244017216"/>
+        <c:axId val="136510424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18560,7 +18563,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244017608"/>
+        <c:crossAx val="136510816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18568,7 +18571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244017608"/>
+        <c:axId val="136510816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -18621,7 +18624,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244017216"/>
+        <c:crossAx val="136510424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -18813,7 +18816,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -18964,7 +18966,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -19035,11 +19036,11 @@
         </c:dLbls>
         <c:gapWidth val="115"/>
         <c:overlap val="-20"/>
-        <c:axId val="244018392"/>
-        <c:axId val="244018784"/>
+        <c:axId val="136511600"/>
+        <c:axId val="136511992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244018392"/>
+        <c:axId val="136511600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19082,7 +19083,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244018784"/>
+        <c:crossAx val="136511992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -19090,7 +19091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244018784"/>
+        <c:axId val="136511992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -19143,7 +19144,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244018392"/>
+        <c:crossAx val="136511600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -19158,7 +19159,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -41909,7 +41909,7 @@
   <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43022,7 +43022,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45426,7 +45426,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45643,6 +45643,517 @@
       </c>
       <c r="E21">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I2" t="s">
+        <v>238</v>
+      </c>
+      <c r="L2" t="s">
+        <v>234</v>
+      </c>
+      <c r="M2" t="s">
+        <v>231</v>
+      </c>
+      <c r="N2" t="s">
+        <v>232</v>
+      </c>
+      <c r="O2" t="s">
+        <v>233</v>
+      </c>
+      <c r="P2" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>236</v>
+      </c>
+      <c r="R2" t="s">
+        <v>237</v>
+      </c>
+      <c r="S2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>2</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B3:B8)</f>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:J12" si="0">AVERAGE(C3:C8)</f>
+        <v>1.5</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="K12:S12" si="1">AVERAGE(L3:L8)</f>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>2.1666666666666665</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="1"/>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13">
+        <f>STDEV(B3:B8)</f>
+        <v>0.75277265270908089</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:J13" si="2">STDEV(C3:C8)</f>
+        <v>0.83666002653407556</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>0.81649658092772637</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>1.211060141638997</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0.51639777949432275</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>0.81649658092772637</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0.51639777949432275</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ref="K13:S13" si="3">STDEV(L3:L8)</f>
+        <v>0.75277265270908089</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.83666002653407556</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="3"/>
+        <v>0.81649658092772637</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>0.83666002653407556</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="3"/>
+        <v>0.75277265270908089</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>1.0488088481701516</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="3"/>
+        <v>0.40824829046386274</v>
       </c>
     </row>
   </sheetData>
@@ -47781,7 +48292,7 @@
   <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48916,7 +49427,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49535,7 +50046,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="N2" sqref="N2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50531,7 +51042,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50980,7 +51491,7 @@
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="N2" sqref="N2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51892,7 +52403,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52343,8 +52854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>